<commit_message>
finished trainin some of model results for first time, target_col == previous_concussions
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifierDecisionTreeClassifier_randomsearch-estimator_df.xlsx
+++ b/results/AdaBoostClassifierDecisionTreeClassifier_randomsearch-estimator_df.xlsx
@@ -486,23 +486,53 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', None),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'D...
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=1,
-                                                                     min_samples_split=6,
+                                                                     criterion='entropy',
+                                                                     max_depth=5,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=5,
+                                                                     min_samples_split=5,
                                                                      random_state=42),
                                     n_estimators=10, random_state=42))])</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': None, 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 1, 'model__estimator__max_features': None, 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6229976621395386</v>
+        <v>0.6377634051684395</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -513,10 +543,10 @@
         <v>42</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8506876719179794</v>
+        <v>0.9147013644167344</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3782608695652174</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -525,7 +555,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[0 1 1 0 1 0 1 0 0 1 1 0 0 1 0 0 1 0 1 0 0 0 1 1]</t>
+          <t>[0 1 1 0 1 0 1 0 0 0 1 0 1 1 1 0 1 1 1 0 1 0 1 1]</t>
         </is>
       </c>
     </row>
@@ -558,9 +588,9 @@
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
                                                                      criterion='entropy',
-                                                                     max_depth=3,
+                                                                     max_depth=4,
                                                                      max_features='log2',
-                                                                     min_samples_leaf=3,
+                                                                     min_samples_split=5,
                                                                      random_state=42),
                                     n_estimators=10, random_state=42))])</t>
         </is>
@@ -577,11 +607,11 @@
                                   'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
                                   'Delta_RT', 'FullPath_HR', 'FullPath_V',
                                   'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
-                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 2, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 3, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 1, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6076626199887069</v>
+        <v>0.6131014492753624</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -595,7 +625,7 @@
         <v>0.8826267869649405</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3518518518518519</v>
+        <v>0.4611992945326279</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -604,7 +634,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[0 1 1 0 0 1 1 1 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0]</t>
+          <t>[1 0 1 1 1 1 1 0 0 1 0 0 0 0 0 1 1 1 1 0 0 1 0 1]</t>
         </is>
       </c>
     </row>
@@ -660,7 +690,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.5769057921483551</v>
+        <v>0.5676430548856178</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -743,26 +773,53 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', None),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'D...
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     criterion='entropy',
-                                                                     max_depth=6,
-                                                                     max_features='sqrt',
-                                                                     min_samples_leaf=5,
-                                                                     min_samples_split=6,
+                                                                     max_depth=5,
+                                                                     max_features='log2',
+                                                                     min_samples_leaf=4,
+                                                                     min_samples_split=5,
                                                                      random_state=42),
                                     n_estimators=10, random_state=42))])</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': None, 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.5780350278936898</v>
+        <v>0.5812623703527593</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -776,7 +833,7 @@
         <v>0.9147013644167344</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4611992945326279</v>
+        <v>0.5</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -785,7 +842,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[0 1 1 0 0 0 1 0 1 0 0 1 1 1 1 0 0 0 1 1 1 1 1 0]</t>
+          <t>[0 0 0 1 0 0 0 0 1 1 1 1 1 1 1 0 0 0 0 0 0 1 1 0]</t>
         </is>
       </c>
     </row>

</xml_diff>